<commit_message>
fixed accuracy reporting in excel
</commit_message>
<xml_diff>
--- a/Logs/ModelStatistics_03-2024.xlsx
+++ b/Logs/ModelStatistics_03-2024.xlsx
@@ -10580,7 +10580,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK30"/>
+  <dimension ref="A1:AK35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -14052,6 +14052,571 @@
         <v>0.1205427205513733</v>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>50</v>
+      </c>
+      <c r="B31" t="n">
+        <v>30</v>
+      </c>
+      <c r="C31" t="n">
+        <v>150</v>
+      </c>
+      <c r="D31" t="n">
+        <v>13</v>
+      </c>
+      <c r="E31" t="n">
+        <v>12</v>
+      </c>
+      <c r="F31" t="n">
+        <v>150</v>
+      </c>
+      <c r="G31" t="n">
+        <v>41841</v>
+      </c>
+      <c r="H31" t="n">
+        <v>13947</v>
+      </c>
+      <c r="I31" t="n">
+        <v>0.9579837957983796</v>
+      </c>
+      <c r="J31" t="n">
+        <v>1.00516240051624</v>
+      </c>
+      <c r="K31" t="n">
+        <v>0.9579837957983796</v>
+      </c>
+      <c r="L31" t="n">
+        <v>1.00516240051624</v>
+      </c>
+      <c r="M31" t="n">
+        <v>0.2870004092211158</v>
+      </c>
+      <c r="N31" t="n">
+        <v>0.5585626771509554</v>
+      </c>
+      <c r="O31" t="n">
+        <v>0.2565821911054137</v>
+      </c>
+      <c r="P31" t="n">
+        <v>0.3078111996195458</v>
+      </c>
+      <c r="Q31" t="n">
+        <v>0.2850029874526986</v>
+      </c>
+      <c r="R31" t="n">
+        <v>0.2542869092429946</v>
+      </c>
+      <c r="S31" t="n">
+        <v>0.5102040816326531</v>
+      </c>
+      <c r="T31" t="n">
+        <v>0.2092492149586069</v>
+      </c>
+      <c r="U31" t="n">
+        <v>0.2797909407665505</v>
+      </c>
+      <c r="V31" t="n">
+        <v>0.2676737160120846</v>
+      </c>
+      <c r="W31" t="n">
+        <v>0.3545565354556535</v>
+      </c>
+      <c r="X31" t="n">
+        <v>0.3391974749620864</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>0.3637693123023797</v>
+      </c>
+      <c r="Z31" t="n">
+        <v>0.3145479314547932</v>
+      </c>
+      <c r="AA31" t="n">
+        <v>0.3021593570423439</v>
+      </c>
+      <c r="AB31" t="n">
+        <v>0.3238684864749717</v>
+      </c>
+      <c r="AC31" t="n">
+        <v>0.9858776361332687</v>
+      </c>
+      <c r="AD31" t="n">
+        <v>0.9839728890099751</v>
+      </c>
+      <c r="AE31" t="n">
+        <v>0.9854987624010469</v>
+      </c>
+      <c r="AF31" t="n">
+        <v>0.9837008942879621</v>
+      </c>
+      <c r="AG31" t="n">
+        <v>0.1753825463130961</v>
+      </c>
+      <c r="AH31" t="n">
+        <v>0.2606212446401409</v>
+      </c>
+      <c r="AI31" t="n">
+        <v>0.2420723124750055</v>
+      </c>
+      <c r="AJ31" t="n">
+        <v>0.2012425656450529</v>
+      </c>
+      <c r="AK31" t="n">
+        <v>0.1206813309266997</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>50</v>
+      </c>
+      <c r="B32" t="n">
+        <v>30</v>
+      </c>
+      <c r="C32" t="n">
+        <v>150</v>
+      </c>
+      <c r="D32" t="n">
+        <v>13</v>
+      </c>
+      <c r="E32" t="n">
+        <v>12</v>
+      </c>
+      <c r="F32" t="n">
+        <v>150</v>
+      </c>
+      <c r="G32" t="n">
+        <v>41841</v>
+      </c>
+      <c r="H32" t="n">
+        <v>13947</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0.9579837957983796</v>
+      </c>
+      <c r="J32" t="n">
+        <v>1.00516240051624</v>
+      </c>
+      <c r="K32" t="n">
+        <v>0.9579837957983796</v>
+      </c>
+      <c r="L32" t="n">
+        <v>1.00516240051624</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0.2870004092211158</v>
+      </c>
+      <c r="N32" t="n">
+        <v>0.5585626771509554</v>
+      </c>
+      <c r="O32" t="n">
+        <v>0.2565821911054137</v>
+      </c>
+      <c r="P32" t="n">
+        <v>0.3078111996195458</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>0.2850029874526986</v>
+      </c>
+      <c r="R32" t="n">
+        <v>0.2542869092429946</v>
+      </c>
+      <c r="S32" t="n">
+        <v>0.5102040816326531</v>
+      </c>
+      <c r="T32" t="n">
+        <v>0.2092492149586069</v>
+      </c>
+      <c r="U32" t="n">
+        <v>0.2797909407665505</v>
+      </c>
+      <c r="V32" t="n">
+        <v>0.2676737160120846</v>
+      </c>
+      <c r="W32" t="n">
+        <v>0.3545565354556535</v>
+      </c>
+      <c r="X32" t="n">
+        <v>0.3391974749620864</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>0.3637693123023797</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>0.3145479314547932</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>0.3021593570423439</v>
+      </c>
+      <c r="AB32" t="n">
+        <v>0.3238684864749717</v>
+      </c>
+      <c r="AC32" t="n">
+        <v>0.9858776361332687</v>
+      </c>
+      <c r="AD32" t="n">
+        <v>0.9839728890099751</v>
+      </c>
+      <c r="AE32" t="n">
+        <v>0.9854987624010469</v>
+      </c>
+      <c r="AF32" t="n">
+        <v>0.9837008942879621</v>
+      </c>
+      <c r="AG32" t="n">
+        <v>0.1753825463130961</v>
+      </c>
+      <c r="AH32" t="n">
+        <v>0.2606212446401409</v>
+      </c>
+      <c r="AI32" t="n">
+        <v>0.2420723124750055</v>
+      </c>
+      <c r="AJ32" t="n">
+        <v>0.2012425656450529</v>
+      </c>
+      <c r="AK32" t="n">
+        <v>0.1206813309266997</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>50</v>
+      </c>
+      <c r="B33" t="n">
+        <v>30</v>
+      </c>
+      <c r="C33" t="n">
+        <v>150</v>
+      </c>
+      <c r="D33" t="n">
+        <v>13</v>
+      </c>
+      <c r="E33" t="n">
+        <v>12</v>
+      </c>
+      <c r="F33" t="n">
+        <v>150</v>
+      </c>
+      <c r="G33" t="n">
+        <v>41841</v>
+      </c>
+      <c r="H33" t="n">
+        <v>13947</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0.9579837957983796</v>
+      </c>
+      <c r="J33" t="n">
+        <v>1.00516240051624</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0.9579837957983796</v>
+      </c>
+      <c r="L33" t="n">
+        <v>1.00516240051624</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0.2870004092211158</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0.5585626771509554</v>
+      </c>
+      <c r="O33" t="n">
+        <v>0.2565821911054137</v>
+      </c>
+      <c r="P33" t="n">
+        <v>0.3078111996195458</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>0.2850029874526986</v>
+      </c>
+      <c r="R33" t="n">
+        <v>0.2542869092429946</v>
+      </c>
+      <c r="S33" t="n">
+        <v>0.5102040816326531</v>
+      </c>
+      <c r="T33" t="n">
+        <v>0.2092492149586069</v>
+      </c>
+      <c r="U33" t="n">
+        <v>0.2797909407665505</v>
+      </c>
+      <c r="V33" t="n">
+        <v>0.2676737160120846</v>
+      </c>
+      <c r="W33" t="n">
+        <v>0.3545565354556535</v>
+      </c>
+      <c r="X33" t="n">
+        <v>0.3391974749620864</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>0.3637693123023797</v>
+      </c>
+      <c r="Z33" t="n">
+        <v>0.3145479314547932</v>
+      </c>
+      <c r="AA33" t="n">
+        <v>0.3021593570423439</v>
+      </c>
+      <c r="AB33" t="n">
+        <v>0.3238684864749717</v>
+      </c>
+      <c r="AC33" t="n">
+        <v>0.9858776361332687</v>
+      </c>
+      <c r="AD33" t="n">
+        <v>0.9839728890099751</v>
+      </c>
+      <c r="AE33" t="n">
+        <v>0.9854987624010469</v>
+      </c>
+      <c r="AF33" t="n">
+        <v>0.9837008942879621</v>
+      </c>
+      <c r="AG33" t="n">
+        <v>0.1753825463130961</v>
+      </c>
+      <c r="AH33" t="n">
+        <v>0.2606212446401409</v>
+      </c>
+      <c r="AI33" t="n">
+        <v>0.2420723124750055</v>
+      </c>
+      <c r="AJ33" t="n">
+        <v>0.2012425656450529</v>
+      </c>
+      <c r="AK33" t="n">
+        <v>0.1206813309266997</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>50</v>
+      </c>
+      <c r="B34" t="n">
+        <v>30</v>
+      </c>
+      <c r="C34" t="n">
+        <v>150</v>
+      </c>
+      <c r="D34" t="n">
+        <v>13</v>
+      </c>
+      <c r="E34" t="n">
+        <v>12</v>
+      </c>
+      <c r="F34" t="n">
+        <v>150</v>
+      </c>
+      <c r="G34" t="n">
+        <v>41841</v>
+      </c>
+      <c r="H34" t="n">
+        <v>13947</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0.9579837957983796</v>
+      </c>
+      <c r="J34" t="n">
+        <v>1.00516240051624</v>
+      </c>
+      <c r="K34" t="n">
+        <v>0.9579837957983796</v>
+      </c>
+      <c r="L34" t="n">
+        <v>1.00516240051624</v>
+      </c>
+      <c r="M34" t="n">
+        <v>0.2870004092211158</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0.5585626771509554</v>
+      </c>
+      <c r="O34" t="n">
+        <v>0.2565821911054137</v>
+      </c>
+      <c r="P34" t="n">
+        <v>0.3078111996195458</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>0.2850029874526986</v>
+      </c>
+      <c r="R34" t="n">
+        <v>0.2542869092429946</v>
+      </c>
+      <c r="S34" t="n">
+        <v>0.5102040816326531</v>
+      </c>
+      <c r="T34" t="n">
+        <v>0.2092492149586069</v>
+      </c>
+      <c r="U34" t="n">
+        <v>0.2797909407665505</v>
+      </c>
+      <c r="V34" t="n">
+        <v>0.2676737160120846</v>
+      </c>
+      <c r="W34" t="n">
+        <v>0.3545565354556535</v>
+      </c>
+      <c r="X34" t="n">
+        <v>0.3391974749620864</v>
+      </c>
+      <c r="Y34" t="n">
+        <v>0.3637693123023797</v>
+      </c>
+      <c r="Z34" t="n">
+        <v>0.3145479314547932</v>
+      </c>
+      <c r="AA34" t="n">
+        <v>0.3021593570423439</v>
+      </c>
+      <c r="AB34" t="n">
+        <v>0.3238684864749717</v>
+      </c>
+      <c r="AC34" t="n">
+        <v>0.9858776361332687</v>
+      </c>
+      <c r="AD34" t="n">
+        <v>0.9839728890099751</v>
+      </c>
+      <c r="AE34" t="n">
+        <v>0.9854987624010469</v>
+      </c>
+      <c r="AF34" t="n">
+        <v>0.9837008942879621</v>
+      </c>
+      <c r="AG34" t="n">
+        <v>0.1753825463130961</v>
+      </c>
+      <c r="AH34" t="n">
+        <v>0.2606212446401409</v>
+      </c>
+      <c r="AI34" t="n">
+        <v>0.2420723124750055</v>
+      </c>
+      <c r="AJ34" t="n">
+        <v>0.2012425656450529</v>
+      </c>
+      <c r="AK34" t="n">
+        <v>0.1206813309266997</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>50</v>
+      </c>
+      <c r="B35" t="n">
+        <v>30</v>
+      </c>
+      <c r="C35" t="n">
+        <v>150</v>
+      </c>
+      <c r="D35" t="n">
+        <v>13</v>
+      </c>
+      <c r="E35" t="n">
+        <v>12</v>
+      </c>
+      <c r="F35" t="n">
+        <v>150</v>
+      </c>
+      <c r="G35" t="n">
+        <v>41841</v>
+      </c>
+      <c r="H35" t="n">
+        <v>13947</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0.3545565354556535</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0.3145479314547932</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0.9579837957983796</v>
+      </c>
+      <c r="L35" t="n">
+        <v>1.00516240051624</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0.2870004092211158</v>
+      </c>
+      <c r="N35" t="n">
+        <v>0.5585626771509554</v>
+      </c>
+      <c r="O35" t="n">
+        <v>0.2565821911054137</v>
+      </c>
+      <c r="P35" t="n">
+        <v>0.3078111996195458</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>0.2850029874526986</v>
+      </c>
+      <c r="R35" t="n">
+        <v>0.2542869092429946</v>
+      </c>
+      <c r="S35" t="n">
+        <v>0.5102040816326531</v>
+      </c>
+      <c r="T35" t="n">
+        <v>0.2092492149586069</v>
+      </c>
+      <c r="U35" t="n">
+        <v>0.2797909407665505</v>
+      </c>
+      <c r="V35" t="n">
+        <v>0.2676737160120846</v>
+      </c>
+      <c r="W35" t="n">
+        <v>0.3545565354556535</v>
+      </c>
+      <c r="X35" t="n">
+        <v>0.3391974749620864</v>
+      </c>
+      <c r="Y35" t="n">
+        <v>0.3637693123023797</v>
+      </c>
+      <c r="Z35" t="n">
+        <v>0.3145479314547932</v>
+      </c>
+      <c r="AA35" t="n">
+        <v>0.3021593570423439</v>
+      </c>
+      <c r="AB35" t="n">
+        <v>0.3238684864749717</v>
+      </c>
+      <c r="AC35" t="n">
+        <v>0.9858776361332687</v>
+      </c>
+      <c r="AD35" t="n">
+        <v>0.9839728890099751</v>
+      </c>
+      <c r="AE35" t="n">
+        <v>0.9854987624010469</v>
+      </c>
+      <c r="AF35" t="n">
+        <v>0.9837008942879621</v>
+      </c>
+      <c r="AG35" t="n">
+        <v>0.1753825463130961</v>
+      </c>
+      <c r="AH35" t="n">
+        <v>0.2606212446401409</v>
+      </c>
+      <c r="AI35" t="n">
+        <v>0.2420723124750055</v>
+      </c>
+      <c r="AJ35" t="n">
+        <v>0.2012425656450529</v>
+      </c>
+      <c r="AK35" t="n">
+        <v>0.1206813309266997</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -14063,7 +14628,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AF9"/>
+  <dimension ref="A1:AF14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -15017,6 +15582,496 @@
         <v>0.1152874812723873</v>
       </c>
     </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>1e-09</v>
+      </c>
+      <c r="B10" t="n">
+        <v>41841</v>
+      </c>
+      <c r="C10" t="n">
+        <v>13947</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1.077101407710141</v>
+      </c>
+      <c r="E10" t="n">
+        <v>1.074352907435291</v>
+      </c>
+      <c r="F10" t="n">
+        <v>1.077101407710141</v>
+      </c>
+      <c r="G10" t="n">
+        <v>1.074352907435291</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.3381530486973128</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.3084941025875468</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.2432698944877231</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.3693972179289026</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.1911969727145987</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.3400250941028858</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.2979024943310657</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.2326577219526121</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.3867595818815331</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.1927492447129909</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0.296049329604933</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0.2897587100826833</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0.2986369665749777</v>
+      </c>
+      <c r="U10" t="n">
+        <v>0.294543629454363</v>
+      </c>
+      <c r="V10" t="n">
+        <v>0.2892997211981692</v>
+      </c>
+      <c r="W10" t="n">
+        <v>0.2976738458851368</v>
+      </c>
+      <c r="X10" t="n">
+        <v>0.977130279771347</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>0.9724836961503029</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>0.9770549720414323</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>0.9724391563805547</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>0.2059997787195946</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>0.221728927785796</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>0.2415648705449465</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>0.2154189416772743</v>
+      </c>
+      <c r="AF10" t="n">
+        <v>0.1152874812723873</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>1e-09</v>
+      </c>
+      <c r="B11" t="n">
+        <v>41841</v>
+      </c>
+      <c r="C11" t="n">
+        <v>13947</v>
+      </c>
+      <c r="D11" t="n">
+        <v>1.077101407710141</v>
+      </c>
+      <c r="E11" t="n">
+        <v>1.074352907435291</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1.077101407710141</v>
+      </c>
+      <c r="G11" t="n">
+        <v>1.074352907435291</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.3381530486973128</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.3084941025875468</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.2432698944877231</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.3693972179289026</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.1911969727145987</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.3400250941028858</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.2979024943310657</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.2326577219526121</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.3867595818815331</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.1927492447129909</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0.296049329604933</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0.2897587100826833</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0.2986369665749777</v>
+      </c>
+      <c r="U11" t="n">
+        <v>0.294543629454363</v>
+      </c>
+      <c r="V11" t="n">
+        <v>0.2892997211981692</v>
+      </c>
+      <c r="W11" t="n">
+        <v>0.2976738458851368</v>
+      </c>
+      <c r="X11" t="n">
+        <v>0.977130279771347</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>0.9724836961503029</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>0.9770549720414323</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>0.9724391563805547</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>0.2059997787195946</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>0.221728927785796</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>0.2415648705449465</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>0.2154189416772743</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>0.1152874812723873</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>1e-09</v>
+      </c>
+      <c r="B12" t="n">
+        <v>41841</v>
+      </c>
+      <c r="C12" t="n">
+        <v>13947</v>
+      </c>
+      <c r="D12" t="n">
+        <v>1.077101407710141</v>
+      </c>
+      <c r="E12" t="n">
+        <v>1.074352907435291</v>
+      </c>
+      <c r="F12" t="n">
+        <v>1.077101407710141</v>
+      </c>
+      <c r="G12" t="n">
+        <v>1.074352907435291</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.3381530486973128</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.3084941025875468</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.2432698944877231</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.3693972179289026</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.1911969727145987</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.3400250941028858</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.2979024943310657</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.2326577219526121</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.3867595818815331</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.1927492447129909</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0.296049329604933</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0.2897587100826833</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0.2986369665749777</v>
+      </c>
+      <c r="U12" t="n">
+        <v>0.294543629454363</v>
+      </c>
+      <c r="V12" t="n">
+        <v>0.2892997211981692</v>
+      </c>
+      <c r="W12" t="n">
+        <v>0.2976738458851368</v>
+      </c>
+      <c r="X12" t="n">
+        <v>0.977130279771347</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>0.9724836961503029</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>0.9770549720414323</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>0.9724391563805547</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>0.2059997787195946</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>0.221728927785796</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>0.2415648705449465</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>0.2154189416772743</v>
+      </c>
+      <c r="AF12" t="n">
+        <v>0.1152874812723873</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>1e-09</v>
+      </c>
+      <c r="B13" t="n">
+        <v>41841</v>
+      </c>
+      <c r="C13" t="n">
+        <v>13947</v>
+      </c>
+      <c r="D13" t="n">
+        <v>1.077101407710141</v>
+      </c>
+      <c r="E13" t="n">
+        <v>1.074352907435291</v>
+      </c>
+      <c r="F13" t="n">
+        <v>1.077101407710141</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1.074352907435291</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.3381530486973128</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.3084941025875468</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.2432698944877231</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.3693972179289026</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.1911969727145987</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.3400250941028858</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.2979024943310657</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.2326577219526121</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.3867595818815331</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0.1927492447129909</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0.296049329604933</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0.2897587100826833</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0.2986369665749777</v>
+      </c>
+      <c r="U13" t="n">
+        <v>0.294543629454363</v>
+      </c>
+      <c r="V13" t="n">
+        <v>0.2892997211981692</v>
+      </c>
+      <c r="W13" t="n">
+        <v>0.2976738458851368</v>
+      </c>
+      <c r="X13" t="n">
+        <v>0.977130279771347</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>0.9724836961503029</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>0.9770549720414323</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>0.9724391563805547</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>0.2059997787195946</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>0.221728927785796</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>0.2415648705449465</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>0.2154189416772743</v>
+      </c>
+      <c r="AF13" t="n">
+        <v>0.1152874812723873</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>1e-09</v>
+      </c>
+      <c r="B14" t="n">
+        <v>41841</v>
+      </c>
+      <c r="C14" t="n">
+        <v>13947</v>
+      </c>
+      <c r="D14" t="n">
+        <v>0.296049329604933</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.294543629454363</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1.077101407710141</v>
+      </c>
+      <c r="G14" t="n">
+        <v>1.074352907435291</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.3381530486973128</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.3084941025875468</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.2432698944877231</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.3693972179289026</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.1911969727145987</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.3400250941028858</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0.2979024943310657</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.2326577219526121</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0.3867595818815331</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0.1927492447129909</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0.296049329604933</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0.2897587100826833</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0.2986369665749777</v>
+      </c>
+      <c r="U14" t="n">
+        <v>0.294543629454363</v>
+      </c>
+      <c r="V14" t="n">
+        <v>0.2892997211981692</v>
+      </c>
+      <c r="W14" t="n">
+        <v>0.2976738458851368</v>
+      </c>
+      <c r="X14" t="n">
+        <v>0.977130279771347</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>0.9724836961503029</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>0.9770549720414323</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>0.9724391563805547</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>0.2059997787195946</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>0.221728927785796</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>0.2415648705449465</v>
+      </c>
+      <c r="AE14" t="n">
+        <v>0.2154189416772743</v>
+      </c>
+      <c r="AF14" t="n">
+        <v>0.1152874812723873</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -15028,7 +16083,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AG9"/>
+  <dimension ref="A1:AG14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -16008,6 +17063,511 @@
         <v>0.2021495413982104</v>
       </c>
       <c r="AG9" t="n">
+        <v>0.1223280866720397</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="B10" t="n">
+        <v>100</v>
+      </c>
+      <c r="C10" t="n">
+        <v>41841</v>
+      </c>
+      <c r="D10" t="n">
+        <v>13947</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.9621662962166296</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.9605649960564996</v>
+      </c>
+      <c r="G10" t="n">
+        <v>0.9621662962166296</v>
+      </c>
+      <c r="H10" t="n">
+        <v>0.9605649960564996</v>
+      </c>
+      <c r="I10" t="n">
+        <v>0.1846951302687219</v>
+      </c>
+      <c r="J10" t="n">
+        <v>0.677882417481942</v>
+      </c>
+      <c r="K10" t="n">
+        <v>0.06419485257864116</v>
+      </c>
+      <c r="L10" t="n">
+        <v>0.4632029485197955</v>
+      </c>
+      <c r="M10" t="n">
+        <v>0.09818761202947621</v>
+      </c>
+      <c r="N10" t="n">
+        <v>0.1802593057298202</v>
+      </c>
+      <c r="O10" t="n">
+        <v>0.6655328798185941</v>
+      </c>
+      <c r="P10" t="n">
+        <v>0.05766485869254925</v>
+      </c>
+      <c r="Q10" t="n">
+        <v>0.4710801393728223</v>
+      </c>
+      <c r="R10" t="n">
+        <v>0.09123867069486405</v>
+      </c>
+      <c r="S10" t="n">
+        <v>0.3300112330011233</v>
+      </c>
+      <c r="T10" t="n">
+        <v>0.2657490027040982</v>
+      </c>
+      <c r="U10" t="n">
+        <v>0.3807143214181598</v>
+      </c>
+      <c r="V10" t="n">
+        <v>0.3215028321502832</v>
+      </c>
+      <c r="W10" t="n">
+        <v>0.2586301923488591</v>
+      </c>
+      <c r="X10" t="n">
+        <v>0.3732918500649582</v>
+      </c>
+      <c r="Y10" t="n">
+        <v>0.9739243934201258</v>
+      </c>
+      <c r="Z10" t="n">
+        <v>0.9655939136777918</v>
+      </c>
+      <c r="AA10" t="n">
+        <v>0.9752589280958007</v>
+      </c>
+      <c r="AB10" t="n">
+        <v>0.9656993219454908</v>
+      </c>
+      <c r="AC10" t="n">
+        <v>0.174216567239052</v>
+      </c>
+      <c r="AD10" t="n">
+        <v>0.2599268841665893</v>
+      </c>
+      <c r="AE10" t="n">
+        <v>0.2413789205241095</v>
+      </c>
+      <c r="AF10" t="n">
+        <v>0.2021495413982104</v>
+      </c>
+      <c r="AG10" t="n">
+        <v>0.1223280866720397</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="B11" t="n">
+        <v>100</v>
+      </c>
+      <c r="C11" t="n">
+        <v>41841</v>
+      </c>
+      <c r="D11" t="n">
+        <v>13947</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.9621662962166296</v>
+      </c>
+      <c r="F11" t="n">
+        <v>0.9605649960564996</v>
+      </c>
+      <c r="G11" t="n">
+        <v>0.9621662962166296</v>
+      </c>
+      <c r="H11" t="n">
+        <v>0.9605649960564996</v>
+      </c>
+      <c r="I11" t="n">
+        <v>0.1846951302687219</v>
+      </c>
+      <c r="J11" t="n">
+        <v>0.677882417481942</v>
+      </c>
+      <c r="K11" t="n">
+        <v>0.06419485257864116</v>
+      </c>
+      <c r="L11" t="n">
+        <v>0.4632029485197955</v>
+      </c>
+      <c r="M11" t="n">
+        <v>0.09818761202947621</v>
+      </c>
+      <c r="N11" t="n">
+        <v>0.1802593057298202</v>
+      </c>
+      <c r="O11" t="n">
+        <v>0.6655328798185941</v>
+      </c>
+      <c r="P11" t="n">
+        <v>0.05766485869254925</v>
+      </c>
+      <c r="Q11" t="n">
+        <v>0.4710801393728223</v>
+      </c>
+      <c r="R11" t="n">
+        <v>0.09123867069486405</v>
+      </c>
+      <c r="S11" t="n">
+        <v>0.3300112330011233</v>
+      </c>
+      <c r="T11" t="n">
+        <v>0.2657490027040982</v>
+      </c>
+      <c r="U11" t="n">
+        <v>0.3807143214181598</v>
+      </c>
+      <c r="V11" t="n">
+        <v>0.3215028321502832</v>
+      </c>
+      <c r="W11" t="n">
+        <v>0.2586301923488591</v>
+      </c>
+      <c r="X11" t="n">
+        <v>0.3732918500649582</v>
+      </c>
+      <c r="Y11" t="n">
+        <v>0.9739243934201258</v>
+      </c>
+      <c r="Z11" t="n">
+        <v>0.9655939136777918</v>
+      </c>
+      <c r="AA11" t="n">
+        <v>0.9752589280958007</v>
+      </c>
+      <c r="AB11" t="n">
+        <v>0.9656993219454908</v>
+      </c>
+      <c r="AC11" t="n">
+        <v>0.174216567239052</v>
+      </c>
+      <c r="AD11" t="n">
+        <v>0.2599268841665893</v>
+      </c>
+      <c r="AE11" t="n">
+        <v>0.2413789205241095</v>
+      </c>
+      <c r="AF11" t="n">
+        <v>0.2021495413982104</v>
+      </c>
+      <c r="AG11" t="n">
+        <v>0.1223280866720397</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="B12" t="n">
+        <v>100</v>
+      </c>
+      <c r="C12" t="n">
+        <v>41841</v>
+      </c>
+      <c r="D12" t="n">
+        <v>13947</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.9621662962166296</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.9605649960564996</v>
+      </c>
+      <c r="G12" t="n">
+        <v>0.9621662962166296</v>
+      </c>
+      <c r="H12" t="n">
+        <v>0.9605649960564996</v>
+      </c>
+      <c r="I12" t="n">
+        <v>0.1846951302687219</v>
+      </c>
+      <c r="J12" t="n">
+        <v>0.677882417481942</v>
+      </c>
+      <c r="K12" t="n">
+        <v>0.06419485257864116</v>
+      </c>
+      <c r="L12" t="n">
+        <v>0.4632029485197955</v>
+      </c>
+      <c r="M12" t="n">
+        <v>0.09818761202947621</v>
+      </c>
+      <c r="N12" t="n">
+        <v>0.1802593057298202</v>
+      </c>
+      <c r="O12" t="n">
+        <v>0.6655328798185941</v>
+      </c>
+      <c r="P12" t="n">
+        <v>0.05766485869254925</v>
+      </c>
+      <c r="Q12" t="n">
+        <v>0.4710801393728223</v>
+      </c>
+      <c r="R12" t="n">
+        <v>0.09123867069486405</v>
+      </c>
+      <c r="S12" t="n">
+        <v>0.3300112330011233</v>
+      </c>
+      <c r="T12" t="n">
+        <v>0.2657490027040982</v>
+      </c>
+      <c r="U12" t="n">
+        <v>0.3807143214181598</v>
+      </c>
+      <c r="V12" t="n">
+        <v>0.3215028321502832</v>
+      </c>
+      <c r="W12" t="n">
+        <v>0.2586301923488591</v>
+      </c>
+      <c r="X12" t="n">
+        <v>0.3732918500649582</v>
+      </c>
+      <c r="Y12" t="n">
+        <v>0.9739243934201258</v>
+      </c>
+      <c r="Z12" t="n">
+        <v>0.9655939136777918</v>
+      </c>
+      <c r="AA12" t="n">
+        <v>0.9752589280958007</v>
+      </c>
+      <c r="AB12" t="n">
+        <v>0.9656993219454908</v>
+      </c>
+      <c r="AC12" t="n">
+        <v>0.174216567239052</v>
+      </c>
+      <c r="AD12" t="n">
+        <v>0.2599268841665893</v>
+      </c>
+      <c r="AE12" t="n">
+        <v>0.2413789205241095</v>
+      </c>
+      <c r="AF12" t="n">
+        <v>0.2021495413982104</v>
+      </c>
+      <c r="AG12" t="n">
+        <v>0.1223280866720397</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="B13" t="n">
+        <v>100</v>
+      </c>
+      <c r="C13" t="n">
+        <v>41841</v>
+      </c>
+      <c r="D13" t="n">
+        <v>13947</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.9621662962166296</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.9605649960564996</v>
+      </c>
+      <c r="G13" t="n">
+        <v>0.9621662962166296</v>
+      </c>
+      <c r="H13" t="n">
+        <v>0.9605649960564996</v>
+      </c>
+      <c r="I13" t="n">
+        <v>0.1846951302687219</v>
+      </c>
+      <c r="J13" t="n">
+        <v>0.677882417481942</v>
+      </c>
+      <c r="K13" t="n">
+        <v>0.06419485257864116</v>
+      </c>
+      <c r="L13" t="n">
+        <v>0.4632029485197955</v>
+      </c>
+      <c r="M13" t="n">
+        <v>0.09818761202947621</v>
+      </c>
+      <c r="N13" t="n">
+        <v>0.1802593057298202</v>
+      </c>
+      <c r="O13" t="n">
+        <v>0.6655328798185941</v>
+      </c>
+      <c r="P13" t="n">
+        <v>0.05766485869254925</v>
+      </c>
+      <c r="Q13" t="n">
+        <v>0.4710801393728223</v>
+      </c>
+      <c r="R13" t="n">
+        <v>0.09123867069486405</v>
+      </c>
+      <c r="S13" t="n">
+        <v>0.3300112330011233</v>
+      </c>
+      <c r="T13" t="n">
+        <v>0.2657490027040982</v>
+      </c>
+      <c r="U13" t="n">
+        <v>0.3807143214181598</v>
+      </c>
+      <c r="V13" t="n">
+        <v>0.3215028321502832</v>
+      </c>
+      <c r="W13" t="n">
+        <v>0.2586301923488591</v>
+      </c>
+      <c r="X13" t="n">
+        <v>0.3732918500649582</v>
+      </c>
+      <c r="Y13" t="n">
+        <v>0.9739243934201258</v>
+      </c>
+      <c r="Z13" t="n">
+        <v>0.9655939136777918</v>
+      </c>
+      <c r="AA13" t="n">
+        <v>0.9752589280958007</v>
+      </c>
+      <c r="AB13" t="n">
+        <v>0.9656993219454908</v>
+      </c>
+      <c r="AC13" t="n">
+        <v>0.174216567239052</v>
+      </c>
+      <c r="AD13" t="n">
+        <v>0.2599268841665893</v>
+      </c>
+      <c r="AE13" t="n">
+        <v>0.2413789205241095</v>
+      </c>
+      <c r="AF13" t="n">
+        <v>0.2021495413982104</v>
+      </c>
+      <c r="AG13" t="n">
+        <v>0.1223280866720397</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="B14" t="n">
+        <v>100</v>
+      </c>
+      <c r="C14" t="n">
+        <v>41841</v>
+      </c>
+      <c r="D14" t="n">
+        <v>13947</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.3300112330011233</v>
+      </c>
+      <c r="F14" t="n">
+        <v>0.3215028321502832</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.9621662962166296</v>
+      </c>
+      <c r="H14" t="n">
+        <v>0.9605649960564996</v>
+      </c>
+      <c r="I14" t="n">
+        <v>0.1846951302687219</v>
+      </c>
+      <c r="J14" t="n">
+        <v>0.677882417481942</v>
+      </c>
+      <c r="K14" t="n">
+        <v>0.06419485257864116</v>
+      </c>
+      <c r="L14" t="n">
+        <v>0.4632029485197955</v>
+      </c>
+      <c r="M14" t="n">
+        <v>0.09818761202947621</v>
+      </c>
+      <c r="N14" t="n">
+        <v>0.1802593057298202</v>
+      </c>
+      <c r="O14" t="n">
+        <v>0.6655328798185941</v>
+      </c>
+      <c r="P14" t="n">
+        <v>0.05766485869254925</v>
+      </c>
+      <c r="Q14" t="n">
+        <v>0.4710801393728223</v>
+      </c>
+      <c r="R14" t="n">
+        <v>0.09123867069486405</v>
+      </c>
+      <c r="S14" t="n">
+        <v>0.3300112330011233</v>
+      </c>
+      <c r="T14" t="n">
+        <v>0.2657490027040982</v>
+      </c>
+      <c r="U14" t="n">
+        <v>0.3807143214181598</v>
+      </c>
+      <c r="V14" t="n">
+        <v>0.3215028321502832</v>
+      </c>
+      <c r="W14" t="n">
+        <v>0.2586301923488591</v>
+      </c>
+      <c r="X14" t="n">
+        <v>0.3732918500649582</v>
+      </c>
+      <c r="Y14" t="n">
+        <v>0.9739243934201258</v>
+      </c>
+      <c r="Z14" t="n">
+        <v>0.9655939136777918</v>
+      </c>
+      <c r="AA14" t="n">
+        <v>0.9752589280958007</v>
+      </c>
+      <c r="AB14" t="n">
+        <v>0.9656993219454908</v>
+      </c>
+      <c r="AC14" t="n">
+        <v>0.174216567239052</v>
+      </c>
+      <c r="AD14" t="n">
+        <v>0.2599268841665893</v>
+      </c>
+      <c r="AE14" t="n">
+        <v>0.2413789205241095</v>
+      </c>
+      <c r="AF14" t="n">
+        <v>0.2021495413982104</v>
+      </c>
+      <c r="AG14" t="n">
         <v>0.1223280866720397</v>
       </c>
     </row>

</xml_diff>

<commit_message>
re-ran, removed commented code, added excel pitcher average output to run when outputing the averages
</commit_message>
<xml_diff>
--- a/Logs/ModelStatistics_03-2024.xlsx
+++ b/Logs/ModelStatistics_03-2024.xlsx
@@ -3140,7 +3140,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AK31"/>
+  <dimension ref="A1:AK35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3590,7 +3590,7 @@
         <v>0.3545804354580435</v>
       </c>
       <c r="J4" t="n">
-        <v>0.3165555316555532</v>
+        <v>0.3164838316483832</v>
       </c>
       <c r="K4" t="n">
         <v>0.9425204942520494</v>
@@ -3623,7 +3623,7 @@
         <v>0.2003434459072696</v>
       </c>
       <c r="U4" t="n">
-        <v>0.3383802816901408</v>
+        <v>0.3380281690140845</v>
       </c>
       <c r="V4" t="n">
         <v>0.1109799291617473</v>
@@ -3638,13 +3638,13 @@
         <v>0.3728384159466904</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.3165555316555532</v>
+        <v>0.3164838316483832</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.2829715349756672</v>
+        <v>0.2829024980409071</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.3350717843232695</v>
+        <v>0.3349986735807151</v>
       </c>
       <c r="AC4" t="n">
         <v>0.9797565572870844</v>
@@ -6723,6 +6723,458 @@
       </c>
       <c r="AK31" t="n">
         <v>0.1196569115234618</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>50</v>
+      </c>
+      <c r="B32" t="n">
+        <v>30</v>
+      </c>
+      <c r="C32" t="n">
+        <v>150</v>
+      </c>
+      <c r="D32" t="n">
+        <v>13</v>
+      </c>
+      <c r="E32" t="n">
+        <v>12</v>
+      </c>
+      <c r="F32" t="n">
+        <v>150</v>
+      </c>
+      <c r="G32" t="n">
+        <v>41841</v>
+      </c>
+      <c r="H32" t="n">
+        <v>13947</v>
+      </c>
+      <c r="I32" t="n">
+        <v>0.3545565354556535</v>
+      </c>
+      <c r="J32" t="n">
+        <v>0.3145479314547932</v>
+      </c>
+      <c r="K32" t="n">
+        <v>0.9579837957983796</v>
+      </c>
+      <c r="L32" t="n">
+        <v>1.00516240051624</v>
+      </c>
+      <c r="M32" t="n">
+        <v>0.2870004092211158</v>
+      </c>
+      <c r="N32" t="n">
+        <v>0.5585626771509554</v>
+      </c>
+      <c r="O32" t="n">
+        <v>0.2565821911054137</v>
+      </c>
+      <c r="P32" t="n">
+        <v>0.3078111996195458</v>
+      </c>
+      <c r="Q32" t="n">
+        <v>0.2850029874526986</v>
+      </c>
+      <c r="R32" t="n">
+        <v>0.2542869092429946</v>
+      </c>
+      <c r="S32" t="n">
+        <v>0.5102040816326531</v>
+      </c>
+      <c r="T32" t="n">
+        <v>0.2092492149586069</v>
+      </c>
+      <c r="U32" t="n">
+        <v>0.2797909407665505</v>
+      </c>
+      <c r="V32" t="n">
+        <v>0.2676737160120846</v>
+      </c>
+      <c r="W32" t="n">
+        <v>0.3545565354556535</v>
+      </c>
+      <c r="X32" t="n">
+        <v>0.3391974749620864</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>0.3637693123023797</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>0.3145479314547932</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>0.3021593570423439</v>
+      </c>
+      <c r="AB32" t="n">
+        <v>0.3238684864749717</v>
+      </c>
+      <c r="AC32" t="n">
+        <v>0.9858776361332687</v>
+      </c>
+      <c r="AD32" t="n">
+        <v>0.9839728890099751</v>
+      </c>
+      <c r="AE32" t="n">
+        <v>0.9854987624010469</v>
+      </c>
+      <c r="AF32" t="n">
+        <v>0.9837008942879621</v>
+      </c>
+      <c r="AG32" t="n">
+        <v>0.1753825463130961</v>
+      </c>
+      <c r="AH32" t="n">
+        <v>0.2606212446401409</v>
+      </c>
+      <c r="AI32" t="n">
+        <v>0.2420723124750055</v>
+      </c>
+      <c r="AJ32" t="n">
+        <v>0.2012425656450529</v>
+      </c>
+      <c r="AK32" t="n">
+        <v>0.1206813309266997</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>50</v>
+      </c>
+      <c r="B33" t="n">
+        <v>30</v>
+      </c>
+      <c r="C33" t="n">
+        <v>150</v>
+      </c>
+      <c r="D33" t="n">
+        <v>12</v>
+      </c>
+      <c r="E33" t="n">
+        <v>12</v>
+      </c>
+      <c r="F33" t="n">
+        <v>150</v>
+      </c>
+      <c r="G33" t="n">
+        <v>41841</v>
+      </c>
+      <c r="H33" t="n">
+        <v>13947</v>
+      </c>
+      <c r="I33" t="n">
+        <v>0.3574962357496236</v>
+      </c>
+      <c r="J33" t="n">
+        <v>0.3198537319853732</v>
+      </c>
+      <c r="K33" t="n">
+        <v>0.9412059941205995</v>
+      </c>
+      <c r="L33" t="n">
+        <v>0.9911808991180899</v>
+      </c>
+      <c r="M33" t="n">
+        <v>0.2948016415868673</v>
+      </c>
+      <c r="N33" t="n">
+        <v>0.5678614208053073</v>
+      </c>
+      <c r="O33" t="n">
+        <v>0.2582535651494433</v>
+      </c>
+      <c r="P33" t="n">
+        <v>0.3453596012342748</v>
+      </c>
+      <c r="Q33" t="n">
+        <v>0.2165935380933386</v>
+      </c>
+      <c r="R33" t="n">
+        <v>0.2408789386401327</v>
+      </c>
+      <c r="S33" t="n">
+        <v>0.5398671096345515</v>
+      </c>
+      <c r="T33" t="n">
+        <v>0.2081620669406929</v>
+      </c>
+      <c r="U33" t="n">
+        <v>0.3218914185639229</v>
+      </c>
+      <c r="V33" t="n">
+        <v>0.1817087845968712</v>
+      </c>
+      <c r="W33" t="n">
+        <v>0.3574962357496236</v>
+      </c>
+      <c r="X33" t="n">
+        <v>0.338070488059514</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>0.3680698961591991</v>
+      </c>
+      <c r="Z33" t="n">
+        <v>0.3198537319853732</v>
+      </c>
+      <c r="AA33" t="n">
+        <v>0.2963929888286317</v>
+      </c>
+      <c r="AB33" t="n">
+        <v>0.3331131942204167</v>
+      </c>
+      <c r="AC33" t="n">
+        <v>0.9836815270474328</v>
+      </c>
+      <c r="AD33" t="n">
+        <v>0.9766532157984606</v>
+      </c>
+      <c r="AE33" t="n">
+        <v>0.9833947966583783</v>
+      </c>
+      <c r="AF33" t="n">
+        <v>0.9760284125929439</v>
+      </c>
+      <c r="AG33" t="n">
+        <v>0.1748231810041467</v>
+      </c>
+      <c r="AH33" t="n">
+        <v>0.2593638512380261</v>
+      </c>
+      <c r="AI33" t="n">
+        <v>0.244140727888587</v>
+      </c>
+      <c r="AJ33" t="n">
+        <v>0.2015834827580967</v>
+      </c>
+      <c r="AK33" t="n">
+        <v>0.1200887571111419</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="n">
+        <v>50</v>
+      </c>
+      <c r="B34" t="n">
+        <v>30</v>
+      </c>
+      <c r="C34" t="n">
+        <v>150</v>
+      </c>
+      <c r="D34" t="n">
+        <v>15</v>
+      </c>
+      <c r="E34" t="n">
+        <v>12</v>
+      </c>
+      <c r="F34" t="n">
+        <v>150</v>
+      </c>
+      <c r="G34" t="n">
+        <v>41841</v>
+      </c>
+      <c r="H34" t="n">
+        <v>13947</v>
+      </c>
+      <c r="I34" t="n">
+        <v>0.3545804354580435</v>
+      </c>
+      <c r="J34" t="n">
+        <v>0.3166272316627232</v>
+      </c>
+      <c r="K34" t="n">
+        <v>0.9425204942520494</v>
+      </c>
+      <c r="L34" t="n">
+        <v>0.9819315981931598</v>
+      </c>
+      <c r="M34" t="n">
+        <v>0.2897158322056834</v>
+      </c>
+      <c r="N34" t="n">
+        <v>0.6029601029601029</v>
+      </c>
+      <c r="O34" t="n">
+        <v>0.2370443349753694</v>
+      </c>
+      <c r="P34" t="n">
+        <v>0.3696244520791375</v>
+      </c>
+      <c r="Q34" t="n">
+        <v>0.1224407868325973</v>
+      </c>
+      <c r="R34" t="n">
+        <v>0.2427101200686106</v>
+      </c>
+      <c r="S34" t="n">
+        <v>0.5575689991636466</v>
+      </c>
+      <c r="T34" t="n">
+        <v>0.2003434459072696</v>
+      </c>
+      <c r="U34" t="n">
+        <v>0.3387323943661972</v>
+      </c>
+      <c r="V34" t="n">
+        <v>0.1109799291617473</v>
+      </c>
+      <c r="W34" t="n">
+        <v>0.3545804354580435</v>
+      </c>
+      <c r="X34" t="n">
+        <v>0.3197117576777097</v>
+      </c>
+      <c r="Y34" t="n">
+        <v>0.3728384159466904</v>
+      </c>
+      <c r="Z34" t="n">
+        <v>0.3166272316627232</v>
+      </c>
+      <c r="AA34" t="n">
+        <v>0.2830373001711283</v>
+      </c>
+      <c r="AB34" t="n">
+        <v>0.3351463062286507</v>
+      </c>
+      <c r="AC34" t="n">
+        <v>0.9797565572870844</v>
+      </c>
+      <c r="AD34" t="n">
+        <v>0.9789337946707127</v>
+      </c>
+      <c r="AE34" t="n">
+        <v>0.9793059704233507</v>
+      </c>
+      <c r="AF34" t="n">
+        <v>0.9794264830728961</v>
+      </c>
+      <c r="AG34" t="n">
+        <v>0.1733614515419123</v>
+      </c>
+      <c r="AH34" t="n">
+        <v>0.2574720728701375</v>
+      </c>
+      <c r="AI34" t="n">
+        <v>0.243424685685736</v>
+      </c>
+      <c r="AJ34" t="n">
+        <v>0.2038567260727902</v>
+      </c>
+      <c r="AK34" t="n">
+        <v>0.1218850638294205</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>50</v>
+      </c>
+      <c r="B35" t="n">
+        <v>30</v>
+      </c>
+      <c r="C35" t="n">
+        <v>150</v>
+      </c>
+      <c r="D35" t="n">
+        <v>13</v>
+      </c>
+      <c r="E35" t="n">
+        <v>12</v>
+      </c>
+      <c r="F35" t="n">
+        <v>150</v>
+      </c>
+      <c r="G35" t="n">
+        <v>41841</v>
+      </c>
+      <c r="H35" t="n">
+        <v>13947</v>
+      </c>
+      <c r="I35" t="n">
+        <v>0.3527401352740135</v>
+      </c>
+      <c r="J35" t="n">
+        <v>0.3167706316770632</v>
+      </c>
+      <c r="K35" t="n">
+        <v>0.9337491933749194</v>
+      </c>
+      <c r="L35" t="n">
+        <v>0.9772710977271097</v>
+      </c>
+      <c r="M35" t="n">
+        <v>0.246147495872317</v>
+      </c>
+      <c r="N35" t="n">
+        <v>0.6185767097966728</v>
+      </c>
+      <c r="O35" t="n">
+        <v>0.2307015829587649</v>
+      </c>
+      <c r="P35" t="n">
+        <v>0.3865131578947368</v>
+      </c>
+      <c r="Q35" t="n">
+        <v>0.1250249650489315</v>
+      </c>
+      <c r="R35" t="n">
+        <v>0.1951915240423798</v>
+      </c>
+      <c r="S35" t="n">
+        <v>0.5654320987654321</v>
+      </c>
+      <c r="T35" t="n">
+        <v>0.1935483870967742</v>
+      </c>
+      <c r="U35" t="n">
+        <v>0.3658360418923799</v>
+      </c>
+      <c r="V35" t="n">
+        <v>0.1228280407429599</v>
+      </c>
+      <c r="W35" t="n">
+        <v>0.3527401352740135</v>
+      </c>
+      <c r="X35" t="n">
+        <v>0.3154364119471501</v>
+      </c>
+      <c r="Y35" t="n">
+        <v>0.3733683183442749</v>
+      </c>
+      <c r="Z35" t="n">
+        <v>0.3167706316770632</v>
+      </c>
+      <c r="AA35" t="n">
+        <v>0.2814685527386217</v>
+      </c>
+      <c r="AB35" t="n">
+        <v>0.3375914725609019</v>
+      </c>
+      <c r="AC35" t="n">
+        <v>0.987461096996439</v>
+      </c>
+      <c r="AD35" t="n">
+        <v>0.9820436717732028</v>
+      </c>
+      <c r="AE35" t="n">
+        <v>0.9870073526087542</v>
+      </c>
+      <c r="AF35" t="n">
+        <v>0.9816712538876716</v>
+      </c>
+      <c r="AG35" t="n">
+        <v>0.1760814942100116</v>
+      </c>
+      <c r="AH35" t="n">
+        <v>0.2590932541327399</v>
+      </c>
+      <c r="AI35" t="n">
+        <v>0.2437585430138087</v>
+      </c>
+      <c r="AJ35" t="n">
+        <v>0.2022762779546864</v>
+      </c>
+      <c r="AK35" t="n">
+        <v>0.1187904306887337</v>
       </c>
     </row>
   </sheetData>
@@ -13190,61 +13642,61 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.3541056220772288</v>
+        <v>0.3541924118898294</v>
       </c>
       <c r="C2" t="n">
-        <v>0.3171124017112402</v>
+        <v>0.3170911728855879</v>
       </c>
       <c r="D2" t="n">
-        <v>0.9482421548242156</v>
+        <v>0.9477271800668358</v>
       </c>
       <c r="E2" t="n">
-        <v>0.9966396596639658</v>
+        <v>0.9957275231021638</v>
       </c>
       <c r="F2" t="n">
-        <v>0.354105622077229</v>
+        <v>0.3541924118898295</v>
       </c>
       <c r="G2" t="n">
-        <v>0.3310322502913391</v>
+        <v>0.3306877541584304</v>
       </c>
       <c r="H2" t="n">
-        <v>0.3672908593323575</v>
+        <v>0.3675521094918608</v>
       </c>
       <c r="I2" t="n">
-        <v>0.3171124017112402</v>
+        <v>0.3170911728855879</v>
       </c>
       <c r="J2" t="n">
-        <v>0.2931521382056169</v>
+        <v>0.2928692149416022</v>
       </c>
       <c r="K2" t="n">
-        <v>0.3313012636594398</v>
+        <v>0.3314318899566348</v>
       </c>
       <c r="L2" t="n">
-        <v>0.9848333592529926</v>
+        <v>0.9847581645604119</v>
       </c>
       <c r="M2" t="n">
-        <v>0.9798371250419602</v>
+        <v>0.9799034506620929</v>
       </c>
       <c r="N2" t="n">
-        <v>0.9848622155396808</v>
+        <v>0.9847374514200574</v>
       </c>
       <c r="O2" t="n">
-        <v>0.9799316693895015</v>
+        <v>0.979964033103721</v>
       </c>
       <c r="P2" t="n">
-        <v>0.1741885226465841</v>
+        <v>0.1742736574254909</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.2592007793108085</v>
+        <v>0.2591933471236853</v>
       </c>
       <c r="R2" t="n">
-        <v>0.2443373351747024</v>
+        <v>0.2442210683618885</v>
       </c>
       <c r="S2" t="n">
-        <v>0.2023490527543153</v>
+        <v>0.2023361951488261</v>
       </c>
       <c r="T2" t="n">
-        <v>0.1199243101135862</v>
+        <v>0.1199757319401054</v>
       </c>
     </row>
     <row r="3">

</xml_diff>